<commit_message>
Add excel sheet creation
</commit_message>
<xml_diff>
--- a/umg_spreadsheets.xlsx
+++ b/umg_spreadsheets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frames" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="106">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -403,14 +403,55 @@
     <t xml:space="preserve">Sniper Rifle</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Cannot </t>
+    <t xml:space="preserve">4+X</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Gains </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Range </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">bonus equal to the height level of the active </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Cannot </t>
     </r>
     <r>
       <rPr>
@@ -429,17 +470,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">and use </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Sniper Rifle</t>
+      <t xml:space="preserve">and use this module</t>
     </r>
     <r>
       <rPr>
@@ -543,7 +574,26 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> in whole straight line. Can shoot only in same </t>
+      <t xml:space="preserve"> in whole straight line, up to </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Range 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Can shoot only in same </t>
     </r>
     <r>
       <rPr>
@@ -584,6 +634,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mechs</t>
     </r>
@@ -621,6 +672,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mechs</t>
     </r>
@@ -650,6 +702,284 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve"> counter.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Inferno</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Deals damage to all </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mechs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in a triangle shape (stopping where there is a change in height) with </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Range 3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Gives the </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mechs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> damaged that way a </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Burning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> counter.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro Cannon</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Push targeted </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> two spaces away from the attacker, in a straight line. If there are multiple possibilities, the directions is chosen by the active player. If it causes the target to run into a wall or another </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, stop it and deal </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2 Damage </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">to both.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase Knife</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">After using this module, active </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> can move up to half of it’s </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Movement </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">value</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rounded up.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">EX Calibre Blade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Drill</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Both target and active </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">gain Stunned</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
@@ -657,8 +987,161 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">counter</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tokens.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Self Destruct Subroutine</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Applies </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Damage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to the target hex and all hexes in </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Range 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">from it. Destroy active </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> after using this module.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracer Scope</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Chose a target in </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Range 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. During this </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Round</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> it can be attacked by friendly </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mechs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> without the need for </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Line of Sight</t>
     </r>
     <r>
       <rPr>
@@ -671,106 +1154,36 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Inferno</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Deals damage to all </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mechs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> in a triangle shape (stopping where there is a change in height) with </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Range 3. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Gives the </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Mechs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> damaged that way a </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Burning</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> counter.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydro Cannon</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Push targeted </t>
+    <t xml:space="preserve">Self-repairing Armor</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Repairs </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2 Damage </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">from active </t>
     </r>
     <r>
       <rPr>
@@ -789,7 +1202,111 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> two spaces away from the attacker, in a straight line. If there are multiple possibilities, the directions is chosen by the active player. If it causes the target to run into a wall or another </t>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Repairing Nanomachines</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Choose friendly </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">up to </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Range 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Repair </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2 Damage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> from it.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Grid Connection</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Puts all </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Energy </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">from the active </t>
     </r>
     <r>
       <rPr>
@@ -808,59 +1325,50 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">, stop it and deal </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2 Damage </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">to both.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase Knife</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">After dealing </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Damage</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, active </t>
+      <t xml:space="preserve"> into </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Energy Grid.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Siphon</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Steals up to </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2 Energy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> from a </t>
     </r>
     <r>
       <rPr>
@@ -879,62 +1387,59 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> can move up to half of it’s </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Movement </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">value</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">rounded up.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">EX Calibre Blade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power Drill</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Both target and active </t>
+      <t xml:space="preserve"> in </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Range 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Experimental Generator</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Deal up to </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Damage to the active </t>
     </r>
     <r>
       <rPr>
@@ -953,107 +1458,268 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">gain Stunned</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">tokens.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Tracer Scope</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Chose a target in </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Range 4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">. During this </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Round</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> it can be attacked by friendly </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mechs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> without the need for </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Line of Sight</t>
+      <t xml:space="preserve">and put same amount of </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Energy </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">on it.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Gravity Field Projector</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Choose target </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">or the topmost level of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Building </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">in </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Range 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Move it to any hex with no </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">in </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Range 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">from the original location.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Power-Saving Mode</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Generate</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 2 Energy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Cannot perform any other </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Action</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> this turn.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Firewall</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Put a </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Burning </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">counter on each of two adjacent hexes. When any </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> passes through of or ends its move on this counter and it doesn’t have a </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Burning </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">counter, move it onto that </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech</t>
     </r>
     <r>
       <rPr>
@@ -1066,36 +1732,17 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Self-repairing Armor</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Repairs </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2 Damage </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">from active </t>
+    <t xml:space="preserve">Direct Connector</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Choose a </t>
     </r>
     <r>
       <rPr>
@@ -1114,40 +1761,78 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Repairing Nanomachines</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Choose friendly </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mech </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">up to </t>
+      <t xml:space="preserve"> in </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Range 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Put a </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Hacked</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> counter on it.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Hacking Drones</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Choose a </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mech</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in </t>
     </r>
     <r>
       <rPr>
@@ -1166,59 +1851,40 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">. Repair </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2 Damage</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> from it.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Grid Connection</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Puts all </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Energy </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">from the active </t>
+      <t xml:space="preserve">. Put a </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Hacked</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> counter on it.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Extinguisher Drones</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Choose a </t>
     </r>
     <r>
       <rPr>
@@ -1236,596 +1902,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> into </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Energy Grid.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Siphon</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Steals up to </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2 Energy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> from a </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mech</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> in </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Range 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Experimental Generator</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Deal up to </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Damage to the active </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mech </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">and put same amount of </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Energy </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">on it.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Gravity Field Projector</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Choose target </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mech </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">or the topmost level of the </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Building </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">in </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Range 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">. Move it to any hex with no </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mech </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">in </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Range 2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">from the original location.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Power-Saving Mode</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Generate</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 2 Energy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">. Cannot perform any other </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Action</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> this turn.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Firewall</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Put a </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Burning </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">counter on each of two adjacent hexes. When any </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mech</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> passes through of or ends its move on this counter and it doesn’t have a </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Burning </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">counter, move it onto that </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mech</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Direct Connector</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Choose a </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mech</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> in </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Range 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">. Put a </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Hacked</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> counter on it.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Hacking Drones</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Choose a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Mech</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> in </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Range 3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">. Put a </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Hacked</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> counter on it.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Extinguisher Drones</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Choose a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Mech</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> in </t>
     </r>
@@ -2213,7 +2289,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2337,17 +2413,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -2633,7 +2698,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2766,10 +2831,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2882,11 +2943,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="1" width="5.42"/>
@@ -3602,11 +3663,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.67"/>
@@ -3955,14 +4016,14 @@
       <c r="D13" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="E13" s="17" t="n">
-        <v>7</v>
+      <c r="E13" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="F13" s="21" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AME13" s="0"/>
       <c r="AMF13" s="0"/>
@@ -3973,7 +4034,7 @@
     </row>
     <row r="14" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="16" t="n">
         <v>5</v>
@@ -3991,7 +4052,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AME14" s="0"/>
       <c r="AMF14" s="0"/>
@@ -4002,7 +4063,7 @@
     </row>
     <row r="15" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="16" t="n">
         <v>6</v>
@@ -4020,7 +4081,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AME15" s="0"/>
       <c r="AMF15" s="0"/>
@@ -4031,7 +4092,7 @@
     </row>
     <row r="16" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="16" t="n">
         <v>2</v>
@@ -4049,7 +4110,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AME16" s="0"/>
       <c r="AMF16" s="0"/>
@@ -4060,7 +4121,7 @@
     </row>
     <row r="17" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B17" s="16" t="n">
         <v>5</v>
@@ -4078,7 +4139,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AME17" s="0"/>
       <c r="AMF17" s="0"/>
@@ -4089,7 +4150,7 @@
     </row>
     <row r="18" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" s="16" t="n">
         <v>2</v>
@@ -4107,7 +4168,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AME18" s="0"/>
       <c r="AMF18" s="0"/>
@@ -4118,7 +4179,7 @@
     </row>
     <row r="19" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" s="16" t="n">
         <v>3</v>
@@ -4136,7 +4197,7 @@
         <v>12</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AME19" s="0"/>
       <c r="AMF19" s="0"/>
@@ -4147,7 +4208,7 @@
     </row>
     <row r="20" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B20" s="16" t="n">
         <v>5</v>
@@ -4164,7 +4225,7 @@
       <c r="F20" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="32" t="s">
         <v>12</v>
       </c>
       <c r="AME20" s="0"/>
@@ -4176,7 +4237,7 @@
     </row>
     <row r="21" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B21" s="16" t="n">
         <v>4</v>
@@ -4194,7 +4255,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AME21" s="0"/>
       <c r="AMF21" s="0"/>
@@ -4204,13 +4265,27 @@
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="30"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="32"/>
+      <c r="A22" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>58</v>
+      </c>
       <c r="AME22" s="0"/>
       <c r="AMF22" s="0"/>
       <c r="AMG22" s="0"/>
@@ -4270,7 +4345,7 @@
       <c r="D26" s="31"/>
       <c r="E26" s="17"/>
       <c r="F26" s="21"/>
-      <c r="G26" s="34"/>
+      <c r="G26" s="33"/>
       <c r="AME26" s="0"/>
       <c r="AMF26" s="0"/>
       <c r="AMG26" s="0"/>
@@ -4455,18 +4530,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ16"/>
+  <dimension ref="A1:AMJ20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="77.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="77.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4503,19 +4578,19 @@
     </row>
     <row r="3" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="35" t="n">
+        <v>59</v>
+      </c>
+      <c r="B3" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="36" t="n">
+      <c r="D3" s="35" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AMC3" s="0"/>
       <c r="AMD3" s="0"/>
@@ -4528,19 +4603,19 @@
     </row>
     <row r="4" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="35" t="n">
+        <v>61</v>
+      </c>
+      <c r="B4" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="36" t="n">
+      <c r="D4" s="35" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="AMC4" s="0"/>
       <c r="AMD4" s="0"/>
@@ -4553,19 +4628,19 @@
     </row>
     <row r="5" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="35" t="n">
+        <v>63</v>
+      </c>
+      <c r="B5" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="36" t="n">
+      <c r="D5" s="35" t="n">
         <v>3</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AMC5" s="0"/>
       <c r="AMD5" s="0"/>
@@ -4578,19 +4653,19 @@
     </row>
     <row r="6" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="35" t="n">
+        <v>65</v>
+      </c>
+      <c r="B6" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="35" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AMC6" s="0"/>
       <c r="AMD6" s="0"/>
@@ -4603,19 +4678,19 @@
     </row>
     <row r="7" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="35" t="n">
+        <v>67</v>
+      </c>
+      <c r="B7" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="35" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AMC7" s="0"/>
       <c r="AMD7" s="0"/>
@@ -4628,19 +4703,19 @@
     </row>
     <row r="8" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="35" t="n">
+        <v>69</v>
+      </c>
+      <c r="B8" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="35" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AMC8" s="0"/>
       <c r="AMD8" s="0"/>
@@ -4653,19 +4728,19 @@
     </row>
     <row r="9" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="35" t="n">
+        <v>71</v>
+      </c>
+      <c r="B9" s="34" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="36" t="n">
+      <c r="D9" s="35" t="n">
         <v>3</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AMC9" s="0"/>
       <c r="AMD9" s="0"/>
@@ -4678,19 +4753,19 @@
     </row>
     <row r="10" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="35" t="n">
+        <v>73</v>
+      </c>
+      <c r="B10" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AMC10" s="0"/>
       <c r="AMD10" s="0"/>
@@ -4703,19 +4778,19 @@
     </row>
     <row r="11" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="35" t="n">
+        <v>75</v>
+      </c>
+      <c r="B11" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="36" t="n">
+      <c r="D11" s="35" t="n">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="AMC11" s="0"/>
       <c r="AMD11" s="0"/>
@@ -4728,19 +4803,19 @@
     </row>
     <row r="12" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="35" t="n">
+        <v>77</v>
+      </c>
+      <c r="B12" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="36" t="n">
+      <c r="D12" s="35" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AMC12" s="0"/>
       <c r="AMD12" s="0"/>
@@ -4753,19 +4828,19 @@
     </row>
     <row r="13" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="35" t="n">
+        <v>79</v>
+      </c>
+      <c r="B13" s="34" t="n">
         <v>5</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="36" t="n">
+      <c r="D13" s="35" t="n">
         <v>3</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AMC13" s="0"/>
       <c r="AMD13" s="0"/>
@@ -4778,19 +4853,19 @@
     </row>
     <row r="14" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="35" t="n">
+        <v>81</v>
+      </c>
+      <c r="B14" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="36" t="n">
+      <c r="D14" s="35" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="AMC14" s="0"/>
       <c r="AMD14" s="0"/>
@@ -4803,9 +4878,9 @@
     </row>
     <row r="15" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="30"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="32"/>
       <c r="AMC15" s="0"/>
       <c r="AMD15" s="0"/>
@@ -4818,9 +4893,9 @@
     </row>
     <row r="16" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="30"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="36"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="32"/>
       <c r="AMC16" s="0"/>
       <c r="AMD16" s="0"/>
@@ -4830,6 +4905,66 @@
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
       <c r="AMJ16" s="0"/>
+    </row>
+    <row r="17" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="30"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="32"/>
+      <c r="AMC17" s="0"/>
+      <c r="AMD17" s="0"/>
+      <c r="AME17" s="0"/>
+      <c r="AMF17" s="0"/>
+      <c r="AMG17" s="0"/>
+      <c r="AMH17" s="0"/>
+      <c r="AMI17" s="0"/>
+      <c r="AMJ17" s="0"/>
+    </row>
+    <row r="18" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="30"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="32"/>
+      <c r="AMC18" s="0"/>
+      <c r="AMD18" s="0"/>
+      <c r="AME18" s="0"/>
+      <c r="AMF18" s="0"/>
+      <c r="AMG18" s="0"/>
+      <c r="AMH18" s="0"/>
+      <c r="AMI18" s="0"/>
+      <c r="AMJ18" s="0"/>
+    </row>
+    <row r="19" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="30"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="32"/>
+      <c r="AMC19" s="0"/>
+      <c r="AMD19" s="0"/>
+      <c r="AME19" s="0"/>
+      <c r="AMF19" s="0"/>
+      <c r="AMG19" s="0"/>
+      <c r="AMH19" s="0"/>
+      <c r="AMI19" s="0"/>
+      <c r="AMJ19" s="0"/>
+    </row>
+    <row r="20" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="30"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="32"/>
+      <c r="AMC20" s="0"/>
+      <c r="AMD20" s="0"/>
+      <c r="AME20" s="0"/>
+      <c r="AMF20" s="0"/>
+      <c r="AMG20" s="0"/>
+      <c r="AMH20" s="0"/>
+      <c r="AMI20" s="0"/>
+      <c r="AMJ20" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4856,11 +4991,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.67"/>
@@ -4902,19 +5037,19 @@
     </row>
     <row r="3" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="35" t="n">
+        <v>83</v>
+      </c>
+      <c r="B3" s="34" t="n">
         <v>3</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="36" t="s">
-        <v>81</v>
+      <c r="D3" s="35" t="s">
+        <v>84</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AMC3" s="0"/>
       <c r="AMD3" s="0"/>
@@ -4927,19 +5062,19 @@
     </row>
     <row r="4" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="35" t="n">
+        <v>86</v>
+      </c>
+      <c r="B4" s="34" t="n">
         <v>5</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="36" t="s">
-        <v>81</v>
+      <c r="D4" s="35" t="s">
+        <v>84</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AMC4" s="0"/>
       <c r="AMD4" s="0"/>
@@ -4952,19 +5087,19 @@
     </row>
     <row r="5" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="35" t="n">
+        <v>88</v>
+      </c>
+      <c r="B5" s="34" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="35" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="AMC5" s="0"/>
       <c r="AMD5" s="0"/>
@@ -4977,19 +5112,19 @@
     </row>
     <row r="6" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" s="35" t="n">
+        <v>90</v>
+      </c>
+      <c r="B6" s="34" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="35" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AMC6" s="0"/>
       <c r="AMD6" s="0"/>
@@ -5002,19 +5137,19 @@
     </row>
     <row r="7" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="35" t="n">
+        <v>92</v>
+      </c>
+      <c r="B7" s="34" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="37" t="s">
-        <v>90</v>
+      <c r="E7" s="36" t="s">
+        <v>93</v>
       </c>
       <c r="AMC7" s="0"/>
       <c r="AMD7" s="0"/>
@@ -5027,19 +5162,19 @@
     </row>
     <row r="8" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="35" t="n">
+        <v>94</v>
+      </c>
+      <c r="B8" s="34" t="n">
         <v>4</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="37" t="s">
-        <v>92</v>
+      <c r="E8" s="36" t="s">
+        <v>95</v>
       </c>
       <c r="AMC8" s="0"/>
       <c r="AMD8" s="0"/>
@@ -5052,19 +5187,19 @@
     </row>
     <row r="9" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="35" t="n">
+        <v>96</v>
+      </c>
+      <c r="B9" s="34" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="37" t="s">
-        <v>94</v>
+      <c r="E9" s="36" t="s">
+        <v>97</v>
       </c>
       <c r="AMC9" s="0"/>
       <c r="AMD9" s="0"/>
@@ -5077,19 +5212,19 @@
     </row>
     <row r="10" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="35" t="n">
+        <v>98</v>
+      </c>
+      <c r="B10" s="34" t="n">
         <v>4</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="37" t="s">
-        <v>96</v>
+      <c r="E10" s="36" t="s">
+        <v>99</v>
       </c>
       <c r="AMC10" s="0"/>
       <c r="AMD10" s="0"/>
@@ -5102,19 +5237,19 @@
     </row>
     <row r="11" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="35" t="n">
+        <v>100</v>
+      </c>
+      <c r="B11" s="34" t="n">
         <v>3</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="37" t="s">
-        <v>98</v>
+      <c r="E11" s="36" t="s">
+        <v>101</v>
       </c>
       <c r="AMC11" s="0"/>
       <c r="AMD11" s="0"/>
@@ -5127,19 +5262,19 @@
     </row>
     <row r="12" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="35" t="n">
+        <v>102</v>
+      </c>
+      <c r="B12" s="34" t="n">
         <v>5</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="37" t="s">
-        <v>100</v>
+      <c r="E12" s="36" t="s">
+        <v>103</v>
       </c>
       <c r="AMC12" s="0"/>
       <c r="AMD12" s="0"/>
@@ -5152,19 +5287,19 @@
     </row>
     <row r="13" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" s="35" t="n">
+        <v>104</v>
+      </c>
+      <c r="B13" s="34" t="n">
         <v>3</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="35" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="AMC13" s="0"/>
       <c r="AMD13" s="0"/>
@@ -5177,10 +5312,10 @@
     </row>
     <row r="14" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="30"/>
-      <c r="B14" s="35"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="16"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
       <c r="AMC14" s="0"/>
       <c r="AMD14" s="0"/>
       <c r="AME14" s="0"/>
@@ -5192,9 +5327,9 @@
     </row>
     <row r="15" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="30"/>
-      <c r="B15" s="35"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="16"/>
-      <c r="D15" s="36"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="32"/>
       <c r="AMC15" s="0"/>
       <c r="AMD15" s="0"/>
@@ -5207,9 +5342,9 @@
     </row>
     <row r="16" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="30"/>
-      <c r="B16" s="35"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="16"/>
-      <c r="D16" s="36"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="32"/>
       <c r="AMC16" s="0"/>
       <c r="AMD16" s="0"/>
@@ -5222,9 +5357,9 @@
     </row>
     <row r="17" s="14" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="30"/>
-      <c r="B17" s="35"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="16"/>
-      <c r="D17" s="36"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="32"/>
       <c r="AMC17" s="0"/>
       <c r="AMD17" s="0"/>

</xml_diff>